<commit_message>
Adams–Bashforth method added, other methods are optimizd; error handlers added; copy by click and copy all points functions added; placeholders fixed
</commit_message>
<xml_diff>
--- a/ПР9-10_Долинний.xlsx
+++ b/ПР9-10_Долинний.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="29">
   <si>
     <t>i</t>
   </si>
@@ -133,6 +133,21 @@
   <si>
     <t>x*y + y^5 - r3(x)</t>
   </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f0</t>
+  </si>
+  <si>
+    <t>d0</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
 </sst>
 </file>
 
@@ -143,12 +158,20 @@
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,79 +359,83 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -835,16 +862,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -953,19 +980,19 @@
         <v>-0.10000004999999962</v>
       </c>
       <c r="E5" s="6">
-        <f t="shared" ref="E5:E13" si="0">$J$1*D5</f>
+        <f t="shared" ref="E5:E12" si="0">$J$1*D5</f>
         <v>-1.0000004999999962E-4</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" ref="F5:F13" si="1">C5+E5</f>
+        <f t="shared" ref="F5:F12" si="1">C5+E5</f>
         <v>-1.5000004999999943E-4</v>
       </c>
       <c r="G5" s="6">
-        <f t="shared" ref="G5:G13" si="2">B6*F5+POWER(F5,5)-POWER(B6,(1/3))</f>
+        <f t="shared" ref="G5:G12" si="2">B6*F5+POWER(F5,5)-POWER(B6,(1/3))</f>
         <v>-0.12599240498958716</v>
       </c>
       <c r="H5" s="6">
-        <f t="shared" ref="H5:H13" si="3">(D5+G5)*$J$1/2</f>
+        <f t="shared" ref="H5:H12" si="3">(D5+G5)*$J$1/2</f>
         <v>-1.1299622749479339E-4</v>
       </c>
     </row>
@@ -977,11 +1004,11 @@
         <v>1.9999999999999901E-3</v>
       </c>
       <c r="C6" s="19">
-        <f t="shared" ref="C6:C14" si="4">C5+H5</f>
+        <f t="shared" ref="C6:C12" si="4">C5+H5</f>
         <v>-1.6299622749479321E-4</v>
       </c>
       <c r="D6" s="6">
-        <f t="shared" ref="D6:D13" si="5">B6*C6+POWER(C6,5)-POWER(B6,1/3)</f>
+        <f t="shared" ref="D6:D12" si="5">B6*C6+POWER(C6,5)-POWER(B6,1/3)</f>
         <v>-0.12599243098194216</v>
       </c>
       <c r="E6" s="6">
@@ -1509,7 +1536,7 @@
         <v>0.02</v>
       </c>
       <c r="N23" s="18">
-        <f t="shared" ref="N23:N31" si="16">N22+S22</f>
+        <f t="shared" ref="N23:N30" si="16">N22+S22</f>
         <v>-7.0391699865838236E-2</v>
       </c>
       <c r="O23" s="11">
@@ -2035,7 +2062,7 @@
         <v>-0.53201699140062664</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="18.75">
+    <row r="36" spans="1:10" ht="18.75">
       <c r="B36" s="1">
         <v>0.1</v>
       </c>
@@ -2055,7 +2082,7 @@
         <v>-0.46415888336127797</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="18.75">
+    <row r="37" spans="1:10" ht="18.75">
       <c r="B37" s="1">
         <v>0.1</v>
       </c>
@@ -2076,7 +2103,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="1:10">
       <c r="D38" s="26">
         <f>B37*C37</f>
         <v>-4.9999999999999818E-6</v>
@@ -2094,7 +2121,7 @@
         <v>-0.46416388336127795</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="18.75">
+    <row r="40" spans="1:10" ht="18.75">
       <c r="B40" s="1">
         <v>1E-3</v>
       </c>
@@ -2115,7 +2142,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="1:10">
       <c r="D41" s="26">
         <f>B40*C40</f>
         <v>-4.9999999999999812E-8</v>
@@ -2132,6 +2159,648 @@
         <f>D41+E41-F41</f>
         <v>-0.10000005000000002</v>
       </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" thickBot="1">
+      <c r="I42" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A43" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A44" s="10">
+        <v>0</v>
+      </c>
+      <c r="B44" s="16">
+        <v>0</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+    </row>
+    <row r="45" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A45" s="10">
+        <v>1</v>
+      </c>
+      <c r="B45" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C45" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D45" s="11">
+        <f>B44</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="11">
+        <f t="shared" ref="E45:E54" si="18">1/2*$J$42*D45</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="11">
+        <f>B45</f>
+        <v>0.1</v>
+      </c>
+      <c r="G45" s="11">
+        <f>3/2*$J$42*F45</f>
+        <v>1.5000000000000003E-2</v>
+      </c>
+      <c r="H45" s="11">
+        <f>G45-E45</f>
+        <v>1.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A46" s="10">
+        <v>2</v>
+      </c>
+      <c r="B46" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="C46" s="18">
+        <f t="shared" ref="C46:C54" si="19">C45+H45</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="D46" s="11">
+        <f t="shared" ref="D46:D54" si="20">B45</f>
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="11">
+        <f t="shared" si="18"/>
+        <v>5.000000000000001E-3</v>
+      </c>
+      <c r="F46" s="11">
+        <f t="shared" ref="F46:F54" si="21">B46</f>
+        <v>0.2</v>
+      </c>
+      <c r="G46" s="11">
+        <f t="shared" ref="G46:G54" si="22">3/2*$J$42*F46</f>
+        <v>3.0000000000000006E-2</v>
+      </c>
+      <c r="H46" s="11">
+        <f t="shared" ref="H46:H54" si="23">G46-E46</f>
+        <v>2.5000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A47" s="10">
+        <v>3</v>
+      </c>
+      <c r="B47" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C47" s="18">
+        <f t="shared" si="19"/>
+        <v>4.5000000000000012E-2</v>
+      </c>
+      <c r="D47" s="11">
+        <f t="shared" si="20"/>
+        <v>0.2</v>
+      </c>
+      <c r="E47" s="11">
+        <f t="shared" si="18"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="21"/>
+        <v>0.3</v>
+      </c>
+      <c r="G47" s="11">
+        <f t="shared" si="22"/>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="H47" s="11">
+        <f t="shared" si="23"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A48" s="10">
+        <v>4</v>
+      </c>
+      <c r="B48" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="C48" s="18">
+        <f t="shared" si="19"/>
+        <v>8.0000000000000016E-2</v>
+      </c>
+      <c r="D48" s="11">
+        <f t="shared" si="20"/>
+        <v>0.3</v>
+      </c>
+      <c r="E48" s="11">
+        <f t="shared" si="18"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F48" s="11">
+        <f t="shared" si="21"/>
+        <v>0.4</v>
+      </c>
+      <c r="G48" s="11">
+        <f t="shared" si="22"/>
+        <v>6.0000000000000012E-2</v>
+      </c>
+      <c r="H48" s="11">
+        <f t="shared" si="23"/>
+        <v>4.5000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A49" s="10">
+        <v>5</v>
+      </c>
+      <c r="B49" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="C49" s="18">
+        <f t="shared" si="19"/>
+        <v>0.12500000000000003</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="20"/>
+        <v>0.4</v>
+      </c>
+      <c r="E49" s="11">
+        <f t="shared" si="18"/>
+        <v>2.0000000000000004E-2</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="21"/>
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="22"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="H49" s="11">
+        <f t="shared" si="23"/>
+        <v>5.5000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A50" s="10">
+        <v>6</v>
+      </c>
+      <c r="B50" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="C50" s="18">
+        <f t="shared" si="19"/>
+        <v>0.18000000000000005</v>
+      </c>
+      <c r="D50" s="11">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="11">
+        <f t="shared" si="18"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F50" s="11">
+        <f t="shared" si="21"/>
+        <v>0.6</v>
+      </c>
+      <c r="G50" s="11">
+        <f t="shared" si="22"/>
+        <v>9.0000000000000011E-2</v>
+      </c>
+      <c r="H50" s="11">
+        <f t="shared" si="23"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A51" s="10">
+        <v>7</v>
+      </c>
+      <c r="B51" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="C51" s="18">
+        <f t="shared" si="19"/>
+        <v>0.24500000000000005</v>
+      </c>
+      <c r="D51" s="11">
+        <f t="shared" si="20"/>
+        <v>0.6</v>
+      </c>
+      <c r="E51" s="11">
+        <f t="shared" si="18"/>
+        <v>0.03</v>
+      </c>
+      <c r="F51" s="11">
+        <f t="shared" si="21"/>
+        <v>0.7</v>
+      </c>
+      <c r="G51" s="11">
+        <f t="shared" si="22"/>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="H51" s="11">
+        <f t="shared" si="23"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A52" s="10">
+        <v>8</v>
+      </c>
+      <c r="B52" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="C52" s="18">
+        <f t="shared" si="19"/>
+        <v>0.32000000000000006</v>
+      </c>
+      <c r="D52" s="11">
+        <f t="shared" si="20"/>
+        <v>0.7</v>
+      </c>
+      <c r="E52" s="11">
+        <f t="shared" si="18"/>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="21"/>
+        <v>0.8</v>
+      </c>
+      <c r="G52" s="11">
+        <f t="shared" si="22"/>
+        <v>0.12000000000000002</v>
+      </c>
+      <c r="H52" s="11">
+        <f t="shared" si="23"/>
+        <v>8.500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A53" s="10">
+        <v>9</v>
+      </c>
+      <c r="B53" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="C53" s="18">
+        <f t="shared" si="19"/>
+        <v>0.40500000000000008</v>
+      </c>
+      <c r="D53" s="11">
+        <f t="shared" si="20"/>
+        <v>0.8</v>
+      </c>
+      <c r="E53" s="11">
+        <f t="shared" si="18"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="F53" s="11">
+        <f t="shared" si="21"/>
+        <v>0.9</v>
+      </c>
+      <c r="G53" s="11">
+        <f t="shared" si="22"/>
+        <v>0.13500000000000004</v>
+      </c>
+      <c r="H53" s="11">
+        <f t="shared" si="23"/>
+        <v>9.5000000000000029E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A54" s="10">
+        <v>10</v>
+      </c>
+      <c r="B54" s="16">
+        <v>1</v>
+      </c>
+      <c r="C54" s="18">
+        <f t="shared" si="19"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="D54" s="11">
+        <f t="shared" si="20"/>
+        <v>0.9</v>
+      </c>
+      <c r="E54" s="11">
+        <f t="shared" si="18"/>
+        <v>4.5000000000000005E-2</v>
+      </c>
+      <c r="F54" s="11">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="G54" s="11">
+        <f t="shared" si="22"/>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="H54" s="11">
+        <f t="shared" si="23"/>
+        <v>0.10500000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1">
+      <c r="I55" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A56" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+    </row>
+    <row r="57" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A57" s="10">
+        <v>0</v>
+      </c>
+      <c r="B57" s="16">
+        <v>0</v>
+      </c>
+      <c r="C57" s="16">
+        <v>0</v>
+      </c>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+    </row>
+    <row r="58" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A58" s="10">
+        <v>1</v>
+      </c>
+      <c r="B58" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C58" s="29">
+        <v>5.1708329999999997E-3</v>
+      </c>
+      <c r="D58" s="11">
+        <f>B57+C57</f>
+        <v>0</v>
+      </c>
+      <c r="E58" s="11"/>
+      <c r="F58" s="17">
+        <f>B58+C58</f>
+        <v>0.10517083300000001</v>
+      </c>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A59" s="10">
+        <v>2</v>
+      </c>
+      <c r="B59" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="C59" s="29">
+        <f>C58+3/2*$J$55*F58-1/2*$J$55*D58</f>
+        <v>2.0946457950000004E-2</v>
+      </c>
+      <c r="D59" s="11">
+        <f t="shared" ref="D59:D67" si="24">B58+C58</f>
+        <v>0.10517083300000001</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="17">
+        <f t="shared" ref="F59:F67" si="25">B59+C59</f>
+        <v>0.22094645795000001</v>
+      </c>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A60" s="10">
+        <v>3</v>
+      </c>
+      <c r="B60" s="16">
+        <v>0.3</v>
+      </c>
+      <c r="C60" s="29">
+        <f t="shared" ref="C60:C67" si="26">C59+3/2*$J$55*F59-1/2*$J$55*D59</f>
+        <v>4.8829884992500017E-2</v>
+      </c>
+      <c r="D60" s="11">
+        <f t="shared" si="24"/>
+        <v>0.22094645795000001</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="17">
+        <f t="shared" si="25"/>
+        <v>0.34882988499250001</v>
+      </c>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+    </row>
+    <row r="61" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A61" s="10">
+        <v>4</v>
+      </c>
+      <c r="B61" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="C61" s="29">
+        <f t="shared" si="26"/>
+        <v>9.0107044843875023E-2</v>
+      </c>
+      <c r="D61" s="11">
+        <f t="shared" si="24"/>
+        <v>0.34882988499250001</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="17">
+        <f t="shared" si="25"/>
+        <v>0.49010704484387502</v>
+      </c>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A62" s="10">
+        <v>5</v>
+      </c>
+      <c r="B62" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="C62" s="29">
+        <f t="shared" si="26"/>
+        <v>0.1461816073208313</v>
+      </c>
+      <c r="D62" s="11">
+        <f t="shared" si="24"/>
+        <v>0.49010704484387502</v>
+      </c>
+      <c r="E62" s="11"/>
+      <c r="F62" s="17">
+        <f t="shared" si="25"/>
+        <v>0.6461816073208313</v>
+      </c>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A63" s="10">
+        <v>6</v>
+      </c>
+      <c r="B63" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="C63" s="29">
+        <f t="shared" si="26"/>
+        <v>0.21860349617676228</v>
+      </c>
+      <c r="D63" s="11">
+        <f t="shared" si="24"/>
+        <v>0.6461816073208313</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="17">
+        <f t="shared" si="25"/>
+        <v>0.81860349617676231</v>
+      </c>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="1:10" ht="19.5" thickBot="1">
+      <c r="A64" s="10">
+        <v>7</v>
+      </c>
+      <c r="B64" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="C64" s="18">
+        <f t="shared" si="26"/>
+        <v>0.30908494023723504</v>
+      </c>
+      <c r="D64" s="11">
+        <f t="shared" si="24"/>
+        <v>0.81860349617676231</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="17">
+        <f t="shared" si="25"/>
+        <v>1.0090849402372351</v>
+      </c>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="65" spans="1:8" ht="19.5" thickBot="1">
+      <c r="A65" s="10">
+        <v>8</v>
+      </c>
+      <c r="B65" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="C65" s="18">
+        <f t="shared" si="26"/>
+        <v>0.41951750646398223</v>
+      </c>
+      <c r="D65" s="11">
+        <f t="shared" si="24"/>
+        <v>1.0090849402372351</v>
+      </c>
+      <c r="E65" s="11"/>
+      <c r="F65" s="17">
+        <f t="shared" si="25"/>
+        <v>1.2195175064639823</v>
+      </c>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+    </row>
+    <row r="66" spans="1:8" ht="19.5" thickBot="1">
+      <c r="A66" s="10">
+        <v>9</v>
+      </c>
+      <c r="B66" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="C66" s="18">
+        <f t="shared" si="26"/>
+        <v>0.55199088542171781</v>
+      </c>
+      <c r="D66" s="11">
+        <f t="shared" si="24"/>
+        <v>1.2195175064639823</v>
+      </c>
+      <c r="E66" s="11"/>
+      <c r="F66" s="17">
+        <f t="shared" si="25"/>
+        <v>1.4519908854217178</v>
+      </c>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+    </row>
+    <row r="67" spans="1:8" ht="19.5" thickBot="1">
+      <c r="A67" s="10">
+        <v>10</v>
+      </c>
+      <c r="B67" s="16">
+        <v>1</v>
+      </c>
+      <c r="C67" s="29">
+        <f t="shared" si="26"/>
+        <v>0.7088136429117764</v>
+      </c>
+      <c r="D67" s="11">
+        <f t="shared" si="24"/>
+        <v>1.4519908854217178</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="17">
+        <f t="shared" si="25"/>
+        <v>1.7088136429117764</v>
+      </c>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>